<commit_message>
Edited code to extract markers (triggers) of interest and get time between beats in terms of triggers. Starting to relabel columns in psychopy data to extract relevant information from there.
</commit_message>
<xml_diff>
--- a/TriggerValueKey.xlsx
+++ b/TriggerValueKey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/chelsie_hart_ucalgary_ca/Documents/1_PhD_Project/Scripting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{C3EDD849-6733-4C0D-B825-7520A2935591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{175AD9D1-C20F-4EC0-A613-45229B31E3E7}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{C3EDD849-6733-4C0D-B825-7520A2935591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9500E0BB-788B-46FD-8175-059D9E7E5532}"/>
   <bookViews>
-    <workbookView xWindow="5052" yWindow="228" windowWidth="11334" windowHeight="13380" xr2:uid="{3433BB3C-EB46-4EAD-9463-265E383182AF}"/>
+    <workbookView xWindow="380" yWindow="370" windowWidth="12660" windowHeight="19980" xr2:uid="{3433BB3C-EB46-4EAD-9463-265E383182AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Type</t>
   </si>
@@ -98,48 +98,15 @@
     <t>when we ask the participant to adjust their seat/posture</t>
   </si>
   <si>
-    <t>160</t>
-  </si>
-  <si>
     <t>task start</t>
   </si>
   <si>
-    <t>165</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>101 through 125</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>1 through 25</t>
-  </si>
-  <si>
     <t>LostSamples: 3</t>
   </si>
   <si>
     <t>time point where some samples were lost</t>
   </si>
   <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>probe intro screen</t>
   </si>
   <si>
@@ -158,9 +125,6 @@
     <t>task trials</t>
   </si>
   <si>
-    <t>161</t>
-  </si>
-  <si>
     <t>end of MCT</t>
   </si>
   <si>
@@ -170,9 +134,6 @@
     <t>practice 'get ready'</t>
   </si>
   <si>
-    <t>150</t>
-  </si>
-  <si>
     <t>pressed 'up' during practice</t>
   </si>
   <si>
@@ -182,16 +143,82 @@
     <t>practice trials</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>pressed 'up' during main trials</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>break screen</t>
+  </si>
+  <si>
+    <t>6 blinks, 0.1 seconds long, 0.05 seconds apart</t>
+  </si>
+  <si>
+    <t>5 blinks, 0.1 seconds long, 0.05 seconds apart</t>
+  </si>
+  <si>
+    <t>4 blinks, 0.1 seconds long, 0.05 seconds apart</t>
+  </si>
+  <si>
+    <t>1 blink, at 0.75 seconds (same time as beat), 0.075 seconds long (same as beat)</t>
+  </si>
+  <si>
+    <t>Corresponding Photodiode Blinks</t>
+  </si>
+  <si>
+    <t>2 blinks, 0.1 seconds long, 0.05 seconds apart</t>
+  </si>
+  <si>
+    <t>1 blink, 0.5 seconds long</t>
+  </si>
+  <si>
+    <t>3 blinks, 0.1 seconds long, 0.05 seconds apart</t>
+  </si>
+  <si>
+    <t>continuously lit until they exit the break screen</t>
+  </si>
+  <si>
+    <t>S160</t>
+  </si>
+  <si>
+    <t>S165</t>
+  </si>
+  <si>
+    <t>S190</t>
+  </si>
+  <si>
+    <t>S101 through S125</t>
+  </si>
+  <si>
+    <t>S180</t>
+  </si>
+  <si>
+    <t>S170</t>
+  </si>
+  <si>
+    <t>S150</t>
+  </si>
+  <si>
+    <t>S40</t>
+  </si>
+  <si>
+    <t>S90</t>
+  </si>
+  <si>
+    <t>S1 through S25</t>
+  </si>
+  <si>
+    <t>S80</t>
+  </si>
+  <si>
+    <t>S70</t>
+  </si>
+  <si>
+    <t>S50</t>
+  </si>
+  <si>
+    <t>S30</t>
+  </si>
+  <si>
+    <t>S161</t>
   </si>
 </sst>
 </file>
@@ -545,20 +572,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31699526-CDC9-4CEC-9C06-026E04BF125D}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.3125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.20703125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.453125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,267 +595,308 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B11" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more script for looking at timing differences in psychopy data between triggers, photodiodes, and stimui; as well as to look at differences within each to see trial time and stimulus length.
</commit_message>
<xml_diff>
--- a/TriggerValueKey.xlsx
+++ b/TriggerValueKey.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="150" documentId="8_{C3EDD849-6733-4C0D-B825-7520A2935591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5973218-22EA-4FDB-931D-46019ACB9042}"/>
   <bookViews>
-    <workbookView xWindow="-19300" yWindow="2240" windowWidth="16150" windowHeight="18080" xr2:uid="{3433BB3C-EB46-4EAD-9463-265E383182AF}"/>
+    <workbookView xWindow="-30400" yWindow="1500" windowWidth="16150" windowHeight="18080" xr2:uid="{3433BB3C-EB46-4EAD-9463-265E383182AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D18" sqref="B18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>